<commit_message>
add average top variance results
</commit_message>
<xml_diff>
--- a/variance/results.xlsx
+++ b/variance/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\DL2020\variance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00142969-CF9A-4706-82F8-EEC0B3FE772C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E831A6F-686F-4FA0-8BD4-A91F59600F2B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{AD9DF136-7893-4F50-9029-003C12B6CF9D}"/>
   </bookViews>
@@ -37,8 +37,8 @@
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId6"/>
     <pivotCache cacheId="1" r:id="rId7"/>
-    <pivotCache cacheId="5" r:id="rId8"/>
-    <pivotCache cacheId="13" r:id="rId9"/>
+    <pivotCache cacheId="2" r:id="rId8"/>
+    <pivotCache cacheId="3" r:id="rId9"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -114,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="64">
   <si>
     <t>Source.Name</t>
   </si>
@@ -301,6 +301,12 @@
   <si>
     <t>Max. von valid_loss</t>
   </si>
+  <si>
+    <t>Mittelwert von valid_loss</t>
+  </si>
+  <si>
+    <t>Mittelwert von train_loss</t>
+  </si>
 </sst>
 </file>
 
@@ -364,7 +370,7 @@
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="47">
     <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
@@ -372,10 +378,106 @@
       <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <numFmt numFmtId="165" formatCode="0.000%"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.000%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
@@ -388,6 +490,18 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="0.000%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
@@ -11919,6 +12033,174 @@
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="7"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="8"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="9"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
       <c:layout>
@@ -11962,7 +12244,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>more_diagrams!$A$2:$A$22</c:f>
+              <c:f>more_diagrams!$A$2:$A$21</c:f>
               <c:strCache>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
@@ -12030,9 +12312,9 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>more_diagrams!$B$2:$B$22</c:f>
+              <c:f>more_diagrams!$B$2:$B$21</c:f>
               <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
+                <c:formatCode>0.000%</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>0.11478747427463531</c:v>
@@ -12112,7 +12394,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Max. von accuracy</c:v>
+                  <c:v>Mittelwert von accuracy</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -12129,7 +12411,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>more_diagrams!$A$2:$A$22</c:f>
+              <c:f>more_diagrams!$A$2:$A$21</c:f>
               <c:strCache>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
@@ -12197,69 +12479,69 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>more_diagrams!$C$2:$C$22</c:f>
+              <c:f>more_diagrams!$C$2:$C$21</c:f>
               <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
+                <c:formatCode>0.000%</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>0.31051158905029297</c:v>
+                  <c:v>0.26002981577600753</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.39577502012252808</c:v>
+                  <c:v>0.34885648829596383</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.39068466424942017</c:v>
+                  <c:v>0.28480529401983534</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.52965128421783447</c:v>
+                  <c:v>0.45450314368520467</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.4810384213924408</c:v>
+                  <c:v>0.35080536774226595</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.61669635772705078</c:v>
+                  <c:v>0.5778787800243923</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.58742684125900269</c:v>
+                  <c:v>0.49558230212756565</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.69406974315643311</c:v>
+                  <c:v>0.65307057244437083</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.68058031797409058</c:v>
+                  <c:v>0.58508526682853701</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.73657417297363281</c:v>
+                  <c:v>0.7080173100743975</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.73733776807785034</c:v>
+                  <c:v>0.64921645181519649</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.76406210660934448</c:v>
+                  <c:v>0.74192633458546231</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.76329857110977173</c:v>
+                  <c:v>0.72494637284960062</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.78849577903747559</c:v>
+                  <c:v>0.76649093287331715</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.79307711124420166</c:v>
+                  <c:v>0.7579900366919381</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.80274879932403564</c:v>
+                  <c:v>0.78355088574545728</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.81089335680007935</c:v>
+                  <c:v>0.77991491556167603</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.81547468900680542</c:v>
+                  <c:v>0.79434970787593295</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.81394755840301514</c:v>
+                  <c:v>0.79000108752931864</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.8134385347366333</c:v>
+                  <c:v>0.79957094873700818</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12279,7 +12561,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Min. von train_loss</c:v>
+                  <c:v>Max. von accuracy</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -12296,7 +12578,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>more_diagrams!$A$2:$A$22</c:f>
+              <c:f>more_diagrams!$A$2:$A$21</c:f>
               <c:strCache>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
@@ -12364,69 +12646,69 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>more_diagrams!$D$2:$D$22</c:f>
+              <c:f>more_diagrams!$D$2:$D$21</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000%</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>1.96715247631073</c:v>
+                  <c:v>0.31051158905029297</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.8635597229003906</c:v>
+                  <c:v>0.39577502012252808</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.7230443954467773</c:v>
+                  <c:v>0.39068466424942017</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.5912814140319824</c:v>
+                  <c:v>0.52965128421783447</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.4079395532608032</c:v>
+                  <c:v>0.4810384213924408</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.2767505645751953</c:v>
+                  <c:v>0.61669635772705078</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.1173410415649414</c:v>
+                  <c:v>0.58742684125900269</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.0113649368286133</c:v>
+                  <c:v>0.69406974315643311</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.90679484605789185</c:v>
+                  <c:v>0.68058031797409058</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.80843627452850342</c:v>
+                  <c:v>0.73657417297363281</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.71486228704452515</c:v>
+                  <c:v>0.73733776807785034</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.62566733360290527</c:v>
+                  <c:v>0.76406210660934448</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.53257668018341064</c:v>
+                  <c:v>0.76329857110977173</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.4538874626159668</c:v>
+                  <c:v>0.78849577903747559</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.37803187966346741</c:v>
+                  <c:v>0.79307711124420166</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.31312882900238037</c:v>
+                  <c:v>0.80274879932403564</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.2609296441078186</c:v>
+                  <c:v>0.81089335680007935</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.23367065191268921</c:v>
+                  <c:v>0.81547468900680542</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.20773923397064209</c:v>
+                  <c:v>0.81394755840301514</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.20240622758865356</c:v>
+                  <c:v>0.8134385347366333</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12446,7 +12728,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Max. von train_loss</c:v>
+                  <c:v>Min. von train_loss</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -12463,7 +12745,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>more_diagrams!$A$2:$A$22</c:f>
+              <c:f>more_diagrams!$A$2:$A$21</c:f>
               <c:strCache>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
@@ -12531,69 +12813,69 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>more_diagrams!$E$2:$E$22</c:f>
+              <c:f>more_diagrams!$E$2:$E$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>2.3788819313049316</c:v>
+                  <c:v>1.96715247631073</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0655484199523926</c:v>
+                  <c:v>1.8635597229003906</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.8619965314865112</c:v>
+                  <c:v>1.7230443954467773</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.7572512626647949</c:v>
+                  <c:v>1.5912814140319824</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.6730505228042603</c:v>
+                  <c:v>1.4079395532608032</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.5764368772506714</c:v>
+                  <c:v>1.2767505645751953</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.4908559322357178</c:v>
+                  <c:v>1.1173410415649414</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.4088969230651855</c:v>
+                  <c:v>1.0113649368286133</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.3606520891189575</c:v>
+                  <c:v>0.90679484605789185</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.3090825080871582</c:v>
+                  <c:v>0.80843627452850342</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.2516977787017822</c:v>
+                  <c:v>0.71486228704452515</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.2028247117996216</c:v>
+                  <c:v>0.62566733360290527</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.1490942239761353</c:v>
+                  <c:v>0.53257668018341064</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.0966407060623169</c:v>
+                  <c:v>0.4538874626159668</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.0412372350692749</c:v>
+                  <c:v>0.37803187966346741</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.0056285858154297</c:v>
+                  <c:v>0.31312882900238037</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.95756149291992188</c:v>
+                  <c:v>0.2609296441078186</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.91565006971359253</c:v>
+                  <c:v>0.23367065191268921</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.88936638832092285</c:v>
+                  <c:v>0.20773923397064209</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.86356616020202637</c:v>
+                  <c:v>0.20240622758865356</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12613,7 +12895,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Min. von valid_loss</c:v>
+                  <c:v>Mittelwert von train_loss</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -12630,7 +12912,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>more_diagrams!$A$2:$A$22</c:f>
+              <c:f>more_diagrams!$A$2:$A$21</c:f>
               <c:strCache>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
@@ -12698,69 +12980,69 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>more_diagrams!$F$2:$F$22</c:f>
+              <c:f>more_diagrams!$F$2:$F$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>1.9630932807922363</c:v>
+                  <c:v>2.0360896791730609</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.7407023906707764</c:v>
+                  <c:v>1.9214129550116403</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.6977373361587524</c:v>
+                  <c:v>1.813591412135533</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.3564565181732178</c:v>
+                  <c:v>1.6744730881282262</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.4859150648117065</c:v>
+                  <c:v>1.4881550175803049</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.1071408987045288</c:v>
+                  <c:v>1.3317492246627807</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.1933351755142212</c:v>
+                  <c:v>1.2006346259798322</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.92185705900192261</c:v>
+                  <c:v>1.0843888316835677</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.95924198627471924</c:v>
+                  <c:v>0.98453422103609356</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.78925949335098267</c:v>
+                  <c:v>0.88859158413750783</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.80303066968917847</c:v>
+                  <c:v>0.80021656921931672</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.71766173839569092</c:v>
+                  <c:v>0.71126833302634107</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.71914446353912354</c:v>
+                  <c:v>0.63155540568487989</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.6730080246925354</c:v>
+                  <c:v>0.55600006154605319</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.66668671369552612</c:v>
+                  <c:v>0.48544769201959881</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.64634007215499878</c:v>
+                  <c:v>0.42461579867771693</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.64903229475021362</c:v>
+                  <c:v>0.37715433665684289</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.63686865568161011</c:v>
+                  <c:v>0.3417820700577327</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.64149725437164307</c:v>
+                  <c:v>0.31635090793882098</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.64022070169448853</c:v>
+                  <c:v>0.3041142680815288</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12780,7 +13062,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Max. von valid_loss</c:v>
+                  <c:v>Max. von train_loss</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -12797,7 +13079,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>more_diagrams!$A$2:$A$22</c:f>
+              <c:f>more_diagrams!$A$2:$A$21</c:f>
               <c:strCache>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
@@ -12865,69 +13147,69 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>more_diagrams!$G$2:$G$22</c:f>
+              <c:f>more_diagrams!$G$2:$G$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>4.0789780616760254</c:v>
+                  <c:v>2.3788819313049316</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.2276363372802734</c:v>
+                  <c:v>2.0655484199523926</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.8848237991333008</c:v>
+                  <c:v>1.8619965314865112</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.9353946447372437</c:v>
+                  <c:v>1.7572512626647949</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.5209107398986816</c:v>
+                  <c:v>1.6730505228042603</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.3863344192504883</c:v>
+                  <c:v>1.5764368772506714</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.4570426940917969</c:v>
+                  <c:v>1.4908559322357178</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.266349196434021</c:v>
+                  <c:v>1.4088969230651855</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.0172390937805176</c:v>
+                  <c:v>1.3606520891189575</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.1609214544296265</c:v>
+                  <c:v>1.3090825080871582</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.9644038677215576</c:v>
+                  <c:v>1.2516977787017822</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.0466030836105347</c:v>
+                  <c:v>1.2028247117996216</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.2707004547119141</c:v>
+                  <c:v>1.1490942239761353</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.95802384614944458</c:v>
+                  <c:v>1.0966407060623169</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.4671632051467896</c:v>
+                  <c:v>1.0412372350692749</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.88049149513244629</c:v>
+                  <c:v>1.0056285858154297</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.2508711814880371</c:v>
+                  <c:v>0.95756149291992188</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.84963274002075195</c:v>
+                  <c:v>0.91565006971359253</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.0669841766357422</c:v>
+                  <c:v>0.88936638832092285</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.8544013500213623</c:v>
+                  <c:v>0.86356616020202637</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12935,6 +13217,513 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000005-7D31-4834-B10B-8FAF67E84D93}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>more_diagrams!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Min. von valid_loss</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>more_diagrams!$A$2:$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>more_diagrams!$H$2:$H$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1.9630932807922363</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.7407023906707764</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6977373361587524</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.3564565181732178</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.4859150648117065</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.1071408987045288</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.1933351755142212</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.92185705900192261</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.95924198627471924</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.78925949335098267</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.80303066968917847</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.71766173839569092</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.71914446353912354</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.6730080246925354</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.66668671369552612</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.64634007215499878</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.64903229475021362</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.63686865568161011</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.64149725437164307</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.64022070169448853</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8AD6-4D94-A3CF-3D2D2A768FD1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>more_diagrams!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mittelwert von valid_loss</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>more_diagrams!$A$2:$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>more_diagrams!$I$2:$I$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>2.2801819188254222</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9106726918901715</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.4309273140771048</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5816889933177403</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.3332674264907838</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.2297845908573695</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.5714966808046613</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0242589286395483</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.2895889690944127</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.8711335267339434</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.0941139595849174</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.77463465929031372</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.84946037190301082</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.72721600532531738</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.77421364443642748</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.69588099718093877</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.71857755524771549</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.67940135172435212</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.70079528944832936</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.67074030126844131</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-8AD6-4D94-A3CF-3D2D2A768FD1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>more_diagrams!$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Max. von valid_loss</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>more_diagrams!$A$2:$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>more_diagrams!$J$2:$J$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>4.0789780616760254</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.2276363372802734</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.8848237991333008</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.9353946447372437</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.5209107398986816</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.3863344192504883</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.4570426940917969</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.266349196434021</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.0172390937805176</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.1609214544296265</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.9644038677215576</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0466030836105347</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.2707004547119141</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.95802384614944458</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.4671632051467896</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.88049149513244629</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.2508711814880371</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.84963274002075195</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.0669841766357422</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.8544013500213623</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-8AD6-4D94-A3CF-3D2D2A768FD1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -13023,7 +13812,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:numFmt formatCode="0.000%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -19318,16 +20107,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>138112</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>885825</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -32806,7 +33595,7 @@
     <dataField name="Mittelwert von accuracy" fld="4" subtotal="average" baseField="0" baseItem="0" numFmtId="10"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="8">
+    <format dxfId="44">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -33110,7 +33899,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AD0CBD77-7A77-490D-B430-13DE538DFDCE}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AD0CBD77-7A77-490D-B430-13DE538DFDCE}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="H3:AR25" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisCol" showAll="0">
@@ -33811,8 +34600,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{18E6AC05-058C-4198-8CE9-3E7CE1FB0AA2}" name="PivotTable2" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1" fieldListSortAscending="1">
-  <location ref="A1:G22" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{18E6AC05-058C-4198-8CE9-3E7CE1FB0AA2}" name="PivotTable2" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1" fieldListSortAscending="1">
+  <location ref="A1:J21" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField showAll="0">
       <items count="36">
@@ -34434,7 +35223,7 @@
   <rowFields count="1">
     <field x="1"/>
   </rowFields>
-  <rowItems count="21">
+  <rowItems count="20">
     <i>
       <x/>
     </i>
@@ -34495,14 +35284,11 @@
     <i>
       <x v="19"/>
     </i>
-    <i t="grand">
-      <x/>
-    </i>
   </rowItems>
   <colFields count="1">
     <field x="-2"/>
   </colFields>
-  <colItems count="6">
+  <colItems count="9">
     <i>
       <x/>
     </i>
@@ -34521,17 +35307,29 @@
     <i i="5">
       <x v="5"/>
     </i>
+    <i i="6">
+      <x v="6"/>
+    </i>
+    <i i="7">
+      <x v="7"/>
+    </i>
+    <i i="8">
+      <x v="8"/>
+    </i>
   </colItems>
-  <dataFields count="6">
-    <dataField name="Min. von accuracy" fld="4" subtotal="min" baseField="1" baseItem="0"/>
-    <dataField name="Max. von accuracy" fld="4" subtotal="max" baseField="1" baseItem="0"/>
+  <dataFields count="9">
+    <dataField name="Min. von accuracy" fld="4" subtotal="min" baseField="1" baseItem="0" numFmtId="165"/>
+    <dataField name="Mittelwert von accuracy" fld="4" subtotal="average" baseField="1" baseItem="7" numFmtId="165"/>
+    <dataField name="Max. von accuracy" fld="4" subtotal="max" baseField="1" baseItem="0" numFmtId="165"/>
     <dataField name="Min. von train_loss" fld="2" subtotal="min" baseField="1" baseItem="0"/>
+    <dataField name="Mittelwert von train_loss" fld="2" subtotal="average" baseField="1" baseItem="7"/>
     <dataField name="Max. von train_loss" fld="2" subtotal="max" baseField="1" baseItem="0"/>
     <dataField name="Min. von valid_loss" fld="3" subtotal="min" baseField="1" baseItem="0"/>
+    <dataField name="Mittelwert von valid_loss" fld="3" subtotal="average" baseField="1" baseItem="7"/>
     <dataField name="Max. von valid_loss" fld="3" subtotal="max" baseField="1" baseItem="0"/>
   </dataFields>
-  <formats count="2">
-    <format dxfId="0">
+  <formats count="3">
+    <format dxfId="41">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -34541,18 +35339,29 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="1">
+    <format dxfId="40">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
+            <x v="2"/>
           </reference>
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
+    <format dxfId="4">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="3" selected="0">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
   </formats>
-  <chartFormats count="6">
+  <chartFormats count="9">
     <chartFormat chart="0" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
@@ -34566,7 +35375,7 @@
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
+            <x v="2"/>
           </reference>
         </references>
       </pivotArea>
@@ -34575,7 +35384,7 @@
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
+            <x v="3"/>
           </reference>
         </references>
       </pivotArea>
@@ -34584,7 +35393,7 @@
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
-            <x v="3"/>
+            <x v="5"/>
           </reference>
         </references>
       </pivotArea>
@@ -34593,7 +35402,7 @@
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
-            <x v="4"/>
+            <x v="6"/>
           </reference>
         </references>
       </pivotArea>
@@ -34602,7 +35411,34 @@
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
-            <x v="5"/>
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="7" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="8" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="9" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="7"/>
           </reference>
         </references>
       </pivotArea>
@@ -34699,7 +35535,7 @@
     <dataField name="Summe von accuracy" fld="4" baseField="0" baseItem="0" numFmtId="165"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="7">
+    <format dxfId="39">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -35183,12 +36019,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{30460701-2C4E-4C1B-930B-D5A8FB698FD4}" name="reuslts_20_epochs" displayName="reuslts_20_epochs" ref="A1:F101" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:F101" xr:uid="{AB5D210C-5C68-4E5B-9CD9-356FC5AD9AC9}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{E4A9F1B1-A714-4399-9282-1BB5EFB86911}" uniqueName="1" name="Source.Name" queryTableFieldId="1" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{E4A9F1B1-A714-4399-9282-1BB5EFB86911}" uniqueName="1" name="Source.Name" queryTableFieldId="1" dataDxfId="46"/>
     <tableColumn id="2" xr3:uid="{1734CDC0-1D16-458F-938B-9CB69035C171}" uniqueName="2" name="epoch" queryTableFieldId="2"/>
     <tableColumn id="3" xr3:uid="{33FFD6D4-F0C1-4AAF-B999-D31EE8EC64C6}" uniqueName="3" name="train_loss" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{9D8DFB53-98C1-4C30-BAD9-24171180FA6C}" uniqueName="4" name="valid_loss" queryTableFieldId="4"/>
     <tableColumn id="5" xr3:uid="{B3BAEC5B-D9CC-4A77-B547-1953D817B160}" uniqueName="5" name="accuracy" queryTableFieldId="5"/>
-    <tableColumn id="6" xr3:uid="{A3D07C10-A75D-4ADC-96D7-842114D7DFC2}" uniqueName="6" name="time" queryTableFieldId="6" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{A3D07C10-A75D-4ADC-96D7-842114D7DFC2}" uniqueName="6" name="time" queryTableFieldId="6" dataDxfId="45"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -35207,12 +36043,12 @@
     <sortCondition ref="E1:E701"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{E723E4E3-DD7F-4E5F-BBF0-BB87A0066E5B}" uniqueName="1" name="Source.Name" queryTableFieldId="1" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{E723E4E3-DD7F-4E5F-BBF0-BB87A0066E5B}" uniqueName="1" name="Source.Name" queryTableFieldId="1" dataDxfId="43"/>
     <tableColumn id="2" xr3:uid="{33247FEC-74B0-4348-A0F2-0A6C6559DF83}" uniqueName="2" name="epoch" queryTableFieldId="2"/>
     <tableColumn id="3" xr3:uid="{AB6AFE32-13A7-4992-82F6-BB98586CBB62}" uniqueName="3" name="train_loss" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{B5CB369E-CA30-45AB-9A94-EF205149BEC5}" uniqueName="4" name="valid_loss" queryTableFieldId="4"/>
     <tableColumn id="5" xr3:uid="{BD7DD46E-4F9D-4FB1-8E25-F794E205CF5E}" uniqueName="5" name="accuracy" queryTableFieldId="5"/>
-    <tableColumn id="6" xr3:uid="{84319990-1C46-4BE8-BFA4-0028E126AB68}" uniqueName="6" name="time" queryTableFieldId="6" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{84319990-1C46-4BE8-BFA4-0028E126AB68}" uniqueName="6" name="time" queryTableFieldId="6" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -35222,12 +36058,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E56F0E72-AA76-44D2-AA2E-36E5025B6DB8}" name="results_5_epochs" displayName="results_5_epochs" ref="A1:F26" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:F26" xr:uid="{F182CBC8-EC41-419A-B0FA-3A5490845BC8}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{23AE8D65-0410-4355-BA0C-574619675108}" uniqueName="1" name="Source.Name" queryTableFieldId="1" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{23AE8D65-0410-4355-BA0C-574619675108}" uniqueName="1" name="Source.Name" queryTableFieldId="1" dataDxfId="38"/>
     <tableColumn id="2" xr3:uid="{70DC126D-D1A5-4124-A52F-F72ED458CA8A}" uniqueName="2" name="epoch" queryTableFieldId="2"/>
     <tableColumn id="3" xr3:uid="{9796699D-694B-49AE-9449-817D6B8D9F4F}" uniqueName="3" name="train_loss" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{87A492B6-AA51-4390-8C52-29084119461A}" uniqueName="4" name="valid_loss" queryTableFieldId="4"/>
-    <tableColumn id="5" xr3:uid="{FE84C305-876F-4C16-BD20-BD89F8012F7E}" uniqueName="5" name="accuracy" queryTableFieldId="5" dataDxfId="5" dataCellStyle="Prozent"/>
-    <tableColumn id="6" xr3:uid="{E0383F1D-0004-4590-97A3-821B9D6E5D4B}" uniqueName="6" name="time" queryTableFieldId="6" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{FE84C305-876F-4C16-BD20-BD89F8012F7E}" uniqueName="5" name="accuracy" queryTableFieldId="5" dataDxfId="37" dataCellStyle="Prozent"/>
+    <tableColumn id="6" xr3:uid="{E0383F1D-0004-4590-97A3-821B9D6E5D4B}" uniqueName="6" name="time" queryTableFieldId="6" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -54589,28 +55425,30 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40A4CA55-4109-4518-90C6-B8CC3BCDB2D7}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="61" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="61" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="62" max="62" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="63" max="63" width="28.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
@@ -54618,502 +55456,668 @@
         <v>57</v>
       </c>
       <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
         <v>56</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>58</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" t="s">
         <v>60</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>59</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>0</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="7">
         <v>0.11478747427463531</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="7">
+        <v>0.26002981577600753</v>
+      </c>
+      <c r="D2" s="7">
         <v>0.31051158905029297</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="1">
         <v>1.96715247631073</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F2" s="1">
+        <v>2.0360896791730609</v>
+      </c>
+      <c r="G2" s="1">
         <v>2.3788819313049316</v>
       </c>
-      <c r="F2" s="1">
+      <c r="H2" s="1">
         <v>1.9630932807922363</v>
       </c>
-      <c r="G2" s="1">
+      <c r="I2" s="1">
+        <v>2.2801819188254222</v>
+      </c>
+      <c r="J2" s="1">
         <v>4.0789780616760254</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="7">
         <v>0.29854923486709595</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="7">
+        <v>0.34885648829596383</v>
+      </c>
+      <c r="D3" s="7">
         <v>0.39577502012252808</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
         <v>1.8635597229003906</v>
       </c>
-      <c r="E3" s="1">
+      <c r="F3" s="1">
+        <v>1.9214129550116403</v>
+      </c>
+      <c r="G3" s="1">
         <v>2.0655484199523926</v>
       </c>
-      <c r="F3" s="1">
+      <c r="H3" s="1">
         <v>1.7407023906707764</v>
       </c>
-      <c r="G3" s="1">
+      <c r="I3" s="1">
+        <v>1.9106726918901715</v>
+      </c>
+      <c r="J3" s="1">
         <v>2.2276363372802734</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>2</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="7">
         <v>0.17892593145370483</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="7">
+        <v>0.28480529401983534</v>
+      </c>
+      <c r="D4" s="7">
         <v>0.39068466424942017</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E4" s="1">
         <v>1.7230443954467773</v>
       </c>
-      <c r="E4" s="1">
+      <c r="F4" s="1">
+        <v>1.813591412135533</v>
+      </c>
+      <c r="G4" s="1">
         <v>1.8619965314865112</v>
       </c>
-      <c r="F4" s="1">
+      <c r="H4" s="1">
         <v>1.6977373361587524</v>
       </c>
-      <c r="G4" s="1">
+      <c r="I4" s="1">
+        <v>2.4309273140771048</v>
+      </c>
+      <c r="J4" s="1">
         <v>3.8848237991333008</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>3</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="7">
         <v>0.37006872892379761</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="7">
+        <v>0.45450314368520467</v>
+      </c>
+      <c r="D5" s="7">
         <v>0.52965128421783447</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <v>1.5912814140319824</v>
       </c>
-      <c r="E5" s="1">
+      <c r="F5" s="1">
+        <v>1.6744730881282262</v>
+      </c>
+      <c r="G5" s="1">
         <v>1.7572512626647949</v>
       </c>
-      <c r="F5" s="1">
+      <c r="H5" s="1">
         <v>1.3564565181732178</v>
       </c>
-      <c r="G5" s="1">
+      <c r="I5" s="1">
+        <v>1.5816889933177403</v>
+      </c>
+      <c r="J5" s="1">
         <v>1.9353946447372437</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>4</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="7">
         <v>0.219394251704216</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="7">
+        <v>0.35080536774226595</v>
+      </c>
+      <c r="D6" s="7">
         <v>0.4810384213924408</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E6" s="1">
         <v>1.4079395532608032</v>
       </c>
-      <c r="E6" s="1">
+      <c r="F6" s="1">
+        <v>1.4881550175803049</v>
+      </c>
+      <c r="G6" s="1">
         <v>1.6730505228042603</v>
       </c>
-      <c r="F6" s="1">
+      <c r="H6" s="1">
         <v>1.4859150648117065</v>
       </c>
-      <c r="G6" s="1">
+      <c r="I6" s="1">
+        <v>2.3332674264907838</v>
+      </c>
+      <c r="J6" s="1">
         <v>5.5209107398986816</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>5</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="7">
         <v>0.51794350147247314</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="7">
+        <v>0.5778787800243923</v>
+      </c>
+      <c r="D7" s="7">
         <v>0.61669635772705078</v>
       </c>
-      <c r="D7" s="1">
+      <c r="E7" s="1">
         <v>1.2767505645751953</v>
       </c>
-      <c r="E7" s="1">
+      <c r="F7" s="1">
+        <v>1.3317492246627807</v>
+      </c>
+      <c r="G7" s="1">
         <v>1.5764368772506714</v>
       </c>
-      <c r="F7" s="1">
+      <c r="H7" s="1">
         <v>1.1071408987045288</v>
       </c>
-      <c r="G7" s="1">
+      <c r="I7" s="1">
+        <v>1.2297845908573695</v>
+      </c>
+      <c r="J7" s="1">
         <v>1.3863344192504883</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>6</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="7">
         <v>0.32807329297065735</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="7">
+        <v>0.49558230212756565</v>
+      </c>
+      <c r="D8" s="7">
         <v>0.58742684125900269</v>
       </c>
-      <c r="D8" s="1">
+      <c r="E8" s="1">
         <v>1.1173410415649414</v>
       </c>
-      <c r="E8" s="1">
+      <c r="F8" s="1">
+        <v>1.2006346259798322</v>
+      </c>
+      <c r="G8" s="1">
         <v>1.4908559322357178</v>
       </c>
-      <c r="F8" s="1">
+      <c r="H8" s="1">
         <v>1.1933351755142212</v>
       </c>
-      <c r="G8" s="1">
+      <c r="I8" s="1">
+        <v>1.5714966808046613</v>
+      </c>
+      <c r="J8" s="1">
         <v>2.4570426940917969</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>7</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="7">
         <v>0.56426572799682617</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="7">
+        <v>0.65307057244437083</v>
+      </c>
+      <c r="D9" s="7">
         <v>0.69406974315643311</v>
       </c>
-      <c r="D9" s="1">
+      <c r="E9" s="1">
         <v>1.0113649368286133</v>
       </c>
-      <c r="E9" s="1">
+      <c r="F9" s="1">
+        <v>1.0843888316835677</v>
+      </c>
+      <c r="G9" s="1">
         <v>1.4088969230651855</v>
       </c>
-      <c r="F9" s="1">
+      <c r="H9" s="1">
         <v>0.92185705900192261</v>
       </c>
-      <c r="G9" s="1">
+      <c r="I9" s="1">
+        <v>1.0242589286395483</v>
+      </c>
+      <c r="J9" s="1">
         <v>1.266349196434021</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>8</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="7">
         <v>0.43497073650360107</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="7">
+        <v>0.58508526682853701</v>
+      </c>
+      <c r="D10" s="7">
         <v>0.68058031797409058</v>
       </c>
-      <c r="D10" s="1">
+      <c r="E10" s="1">
         <v>0.90679484605789185</v>
       </c>
-      <c r="E10" s="1">
+      <c r="F10" s="1">
+        <v>0.98453422103609356</v>
+      </c>
+      <c r="G10" s="1">
         <v>1.3606520891189575</v>
       </c>
-      <c r="F10" s="1">
+      <c r="H10" s="1">
         <v>0.95924198627471924</v>
       </c>
-      <c r="G10" s="1">
+      <c r="I10" s="1">
+        <v>1.2895889690944127</v>
+      </c>
+      <c r="J10" s="1">
         <v>2.0172390937805176</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>9</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="7">
         <v>0.59811657667160034</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="7">
+        <v>0.7080173100743975</v>
+      </c>
+      <c r="D11" s="7">
         <v>0.73657417297363281</v>
       </c>
-      <c r="D11" s="1">
+      <c r="E11" s="1">
         <v>0.80843627452850342</v>
       </c>
-      <c r="E11" s="1">
+      <c r="F11" s="1">
+        <v>0.88859158413750783</v>
+      </c>
+      <c r="G11" s="1">
         <v>1.3090825080871582</v>
       </c>
-      <c r="F11" s="1">
+      <c r="H11" s="1">
         <v>0.78925949335098267</v>
       </c>
-      <c r="G11" s="1">
+      <c r="I11" s="1">
+        <v>0.8711335267339434</v>
+      </c>
+      <c r="J11" s="1">
         <v>1.1609214544296265</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>10</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="7">
         <v>0.43751591444015503</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="7">
+        <v>0.64921645181519649</v>
+      </c>
+      <c r="D12" s="7">
         <v>0.73733776807785034</v>
       </c>
-      <c r="D12" s="1">
+      <c r="E12" s="1">
         <v>0.71486228704452515</v>
       </c>
-      <c r="E12" s="1">
+      <c r="F12" s="1">
+        <v>0.80021656921931672</v>
+      </c>
+      <c r="G12" s="1">
         <v>1.2516977787017822</v>
       </c>
-      <c r="F12" s="1">
+      <c r="H12" s="1">
         <v>0.80303066968917847</v>
       </c>
-      <c r="G12" s="1">
+      <c r="I12" s="1">
+        <v>1.0941139595849174</v>
+      </c>
+      <c r="J12" s="1">
         <v>1.9644038677215576</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>11</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="7">
         <v>0.64545685052871704</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="7">
+        <v>0.74192633458546231</v>
+      </c>
+      <c r="D13" s="7">
         <v>0.76406210660934448</v>
       </c>
-      <c r="D13" s="1">
+      <c r="E13" s="1">
         <v>0.62566733360290527</v>
       </c>
-      <c r="E13" s="1">
+      <c r="F13" s="1">
+        <v>0.71126833302634107</v>
+      </c>
+      <c r="G13" s="1">
         <v>1.2028247117996216</v>
       </c>
-      <c r="F13" s="1">
+      <c r="H13" s="1">
         <v>0.71766173839569092</v>
       </c>
-      <c r="G13" s="1">
+      <c r="I13" s="1">
+        <v>0.77463465929031372</v>
+      </c>
+      <c r="J13" s="1">
         <v>1.0466030836105347</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>12</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="7">
         <v>0.57342833280563354</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="7">
+        <v>0.72494637284960062</v>
+      </c>
+      <c r="D14" s="7">
         <v>0.76329857110977173</v>
       </c>
-      <c r="D14" s="1">
+      <c r="E14" s="1">
         <v>0.53257668018341064</v>
       </c>
-      <c r="E14" s="1">
+      <c r="F14" s="1">
+        <v>0.63155540568487989</v>
+      </c>
+      <c r="G14" s="1">
         <v>1.1490942239761353</v>
       </c>
-      <c r="F14" s="1">
+      <c r="H14" s="1">
         <v>0.71914446353912354</v>
       </c>
-      <c r="G14" s="1">
+      <c r="I14" s="1">
+        <v>0.84946037190301082</v>
+      </c>
+      <c r="J14" s="1">
         <v>1.2707004547119141</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>13</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="7">
         <v>0.66632729768753052</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="7">
+        <v>0.76649093287331715</v>
+      </c>
+      <c r="D15" s="7">
         <v>0.78849577903747559</v>
       </c>
-      <c r="D15" s="1">
+      <c r="E15" s="1">
         <v>0.4538874626159668</v>
       </c>
-      <c r="E15" s="1">
+      <c r="F15" s="1">
+        <v>0.55600006154605319</v>
+      </c>
+      <c r="G15" s="1">
         <v>1.0966407060623169</v>
       </c>
-      <c r="F15" s="1">
+      <c r="H15" s="1">
         <v>0.6730080246925354</v>
       </c>
-      <c r="G15" s="1">
+      <c r="I15" s="1">
+        <v>0.72721600532531738</v>
+      </c>
+      <c r="J15" s="1">
         <v>0.95802384614944458</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>14</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="7">
         <v>0.57317382097244263</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="7">
+        <v>0.7579900366919381</v>
+      </c>
+      <c r="D16" s="7">
         <v>0.79307711124420166</v>
       </c>
-      <c r="D16" s="1">
+      <c r="E16" s="1">
         <v>0.37803187966346741</v>
       </c>
-      <c r="E16" s="1">
+      <c r="F16" s="1">
+        <v>0.48544769201959881</v>
+      </c>
+      <c r="G16" s="1">
         <v>1.0412372350692749</v>
       </c>
-      <c r="F16" s="1">
+      <c r="H16" s="1">
         <v>0.66668671369552612</v>
       </c>
-      <c r="G16" s="1">
+      <c r="I16" s="1">
+        <v>0.77421364443642748</v>
+      </c>
+      <c r="J16" s="1">
         <v>1.4671632051467896</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>15</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="7">
         <v>0.69305169582366943</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="7">
+        <v>0.78355088574545728</v>
+      </c>
+      <c r="D17" s="7">
         <v>0.80274879932403564</v>
       </c>
-      <c r="D17" s="1">
+      <c r="E17" s="1">
         <v>0.31312882900238037</v>
       </c>
-      <c r="E17" s="1">
+      <c r="F17" s="1">
+        <v>0.42461579867771693</v>
+      </c>
+      <c r="G17" s="1">
         <v>1.0056285858154297</v>
       </c>
-      <c r="F17" s="1">
+      <c r="H17" s="1">
         <v>0.64634007215499878</v>
       </c>
-      <c r="G17" s="1">
+      <c r="I17" s="1">
+        <v>0.69588099718093877</v>
+      </c>
+      <c r="J17" s="1">
         <v>0.88049149513244629</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>16</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="7">
         <v>0.56655639410018921</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="7">
+        <v>0.77991491556167603</v>
+      </c>
+      <c r="D18" s="7">
         <v>0.81089335680007935</v>
       </c>
-      <c r="D18" s="1">
+      <c r="E18" s="1">
         <v>0.2609296441078186</v>
       </c>
-      <c r="E18" s="1">
+      <c r="F18" s="1">
+        <v>0.37715433665684289</v>
+      </c>
+      <c r="G18" s="1">
         <v>0.95756149291992188</v>
       </c>
-      <c r="F18" s="1">
+      <c r="H18" s="1">
         <v>0.64903229475021362</v>
       </c>
-      <c r="G18" s="1">
+      <c r="I18" s="1">
+        <v>0.71857755524771549</v>
+      </c>
+      <c r="J18" s="1">
         <v>1.2508711814880371</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>17</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="7">
         <v>0.71239501237869263</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="7">
+        <v>0.79434970787593295</v>
+      </c>
+      <c r="D19" s="7">
         <v>0.81547468900680542</v>
       </c>
-      <c r="D19" s="1">
+      <c r="E19" s="1">
         <v>0.23367065191268921</v>
       </c>
-      <c r="E19" s="1">
+      <c r="F19" s="1">
+        <v>0.3417820700577327</v>
+      </c>
+      <c r="G19" s="1">
         <v>0.91565006971359253</v>
       </c>
-      <c r="F19" s="1">
+      <c r="H19" s="1">
         <v>0.63686865568161011</v>
       </c>
-      <c r="G19" s="1">
+      <c r="I19" s="1">
+        <v>0.67940135172435212</v>
+      </c>
+      <c r="J19" s="1">
         <v>0.84963274002075195</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>18</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="7">
         <v>0.64036649465560913</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="7">
+        <v>0.79000108752931864</v>
+      </c>
+      <c r="D20" s="7">
         <v>0.81394755840301514</v>
       </c>
-      <c r="D20" s="1">
+      <c r="E20" s="1">
         <v>0.20773923397064209</v>
       </c>
-      <c r="E20" s="1">
+      <c r="F20" s="1">
+        <v>0.31635090793882098</v>
+      </c>
+      <c r="G20" s="1">
         <v>0.88936638832092285</v>
       </c>
-      <c r="F20" s="1">
+      <c r="H20" s="1">
         <v>0.64149725437164307</v>
       </c>
-      <c r="G20" s="1">
+      <c r="I20" s="1">
+        <v>0.70079528944832936</v>
+      </c>
+      <c r="J20" s="1">
         <v>1.0669841766357422</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>19</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="7">
         <v>0.71290403604507446</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C21" s="7">
+        <v>0.79957094873700818</v>
+      </c>
+      <c r="D21" s="7">
         <v>0.8134385347366333</v>
       </c>
-      <c r="D21" s="1">
+      <c r="E21" s="1">
         <v>0.20240622758865356</v>
       </c>
-      <c r="E21" s="1">
+      <c r="F21" s="1">
+        <v>0.3041142680815288</v>
+      </c>
+      <c r="G21" s="1">
         <v>0.86356616020202637</v>
       </c>
-      <c r="F21" s="1">
+      <c r="H21" s="1">
         <v>0.64022070169448853</v>
       </c>
-      <c r="G21" s="1">
+      <c r="I21" s="1">
+        <v>0.67074030126844131</v>
+      </c>
+      <c r="J21" s="1">
         <v>0.8544013500213623</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B22" s="1">
-        <v>0.11478747427463531</v>
-      </c>
-      <c r="C22" s="1">
-        <v>0.81547468900680542</v>
-      </c>
-      <c r="D22" s="1">
-        <v>0.20240622758865356</v>
-      </c>
-      <c r="E22" s="1">
-        <v>2.3788819313049316</v>
-      </c>
-      <c r="F22" s="1">
-        <v>0.63686865568161011</v>
-      </c>
-      <c r="G22" s="1">
-        <v>5.5209107398986816</v>
       </c>
     </row>
   </sheetData>

</xml_diff>